<commit_message>
add lecture 10 11
</commit_message>
<xml_diff>
--- a/GroupInfo/Group.xlsx
+++ b/GroupInfo/Group.xlsx
@@ -39,7 +39,7 @@
     <t>黄键熙</t>
   </si>
   <si>
-    <t>池向元</t>
+    <t>池向沅</t>
   </si>
   <si>
     <t>张涓</t>
@@ -66,19 +66,19 @@
     <t>余钊扬</t>
   </si>
   <si>
-    <t>许芮</t>
+    <t>许芮溧</t>
   </si>
   <si>
     <t>李文婷</t>
   </si>
   <si>
-    <t>王绎</t>
+    <t>王铎</t>
   </si>
   <si>
     <t>建筑物违建检查</t>
   </si>
   <si>
-    <t>自己采集（购买硬纸壳搭建）或者提供多期三维点云数据</t>
+    <t>自己采集或者采用提供的多期三维点云数据</t>
   </si>
   <si>
     <t>完成多期数据的采集与配准，通过变化检测获取违建信息</t>
@@ -96,7 +96,7 @@
     <t>李美仪</t>
   </si>
   <si>
-    <t>陈南宇</t>
+    <t>陈南雨</t>
   </si>
   <si>
     <t>杨畅</t>
@@ -177,11 +177,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,31 +199,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,12 +229,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -252,22 +251,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,15 +304,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -311,45 +335,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,43 +351,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -406,139 +519,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -549,6 +548,80 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -570,82 +643,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -654,152 +653,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -819,22 +818,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1193,7 +1186,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
@@ -1209,118 +1202,118 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1" s="5">
         <v>1</v>
       </c>
-      <c r="C1" s="6">
+      <c r="C1" s="5">
         <v>2</v>
       </c>
-      <c r="D1" s="6">
+      <c r="D1" s="5">
         <v>3</v>
       </c>
-      <c r="E1" s="6">
+      <c r="E1" s="5">
         <v>4</v>
       </c>
-      <c r="F1" s="6">
+      <c r="F1" s="5">
         <v>5</v>
       </c>
-      <c r="G1" s="6">
+      <c r="G1" s="5">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" ht="40.5" spans="1:10">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" ht="40.5" spans="1:10">
-      <c r="A3" s="8" t="s">
+    <row r="3" ht="27" spans="1:10">
+      <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="10" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="11" t="s">
         <v>20</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" ht="40.5" spans="1:10">
-      <c r="A4" s="8" t="s">
+    <row r="4" ht="27" spans="1:10">
+      <c r="A4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="11" t="s">
         <v>29</v>
       </c>
       <c r="J4" s="4" t="s">
@@ -1328,63 +1321,63 @@
       </c>
     </row>
     <row r="5" ht="27" spans="1:10">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="11" t="s">
         <v>39</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" ht="40.5" spans="1:10">
-      <c r="A6" s="8" t="s">
+    <row r="6" ht="27" spans="1:10">
+      <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="11" t="s">
         <v>49</v>
       </c>
       <c r="J6" s="4" t="s">

</xml_diff>